<commit_message>
08-02-2016 Changes By Vimal
</commit_message>
<xml_diff>
--- a/20160208-test result-dtd.xlsx
+++ b/20160208-test result-dtd.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Software\Development\xampp\htdocs\dtd\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="19560" windowHeight="7830" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="19560" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,199 +24,199 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
   <si>
     <t>customer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>profile not displayed.
 processing error</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>check the code.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>same id access</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>once log on the system, do not permited same id log-in simultaneously.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">date field should be read-only. </t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>system date default. not editable by customer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>a6@yahoo.com/
 pw 1234</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>all</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>dash board</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">request sent' should be reset after finishing downloading by vendor. </t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">vendor dashboard is working correctly. </t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>delivery request</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>it is for delivery cancelled by the vendor.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>we can access with same id simultaneously.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>zip code</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>import</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>delivery request 'import' button not working</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>excel file columns are same with the screen page.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>pls apply to vendor's downloading excel file format on customer as well as recipient.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>vendor</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>v13@gmail.com
 pass 1234</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>delivery request date not received.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>check the code</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>reports-order page : admin's page mis-linked. 
 today and monthly tables are for the admin not vendor.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>order delete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>when finishing downlonding, order data should not be deleted or edited by the customer. We can delete requested order after processing code received.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">"- add zipcode column to delivery 'request'
  - add zipcode column to customer substription page
 - 5 digits code is necessary
 </t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>message board</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>"- delete button is necessary for 'sent message'
 - 'new message' error code displayed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>reports</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>admin</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>vendor payment</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>"-'paid' code should be automatically generated when payment data is generated.
 - vendor payment list table and downloading button for banking transfer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>approved order</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>"- 'approved order' completion list not found anywhere.
 - customer's current outstanding table is necessary</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>item table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>"- 'selected' option
 - 'display' option</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>we could set up many different item table and need set options.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>excel file format</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>" refer to the format provided with</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>request processed' to 'request cancelled'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>"- admin needs settlement data to input to vendor's account.
 - with some reason, there will be a chance to deduct money to be paid.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>this Is for exceptional transaction adjustment.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>vendor/customer/admin</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>order delivered status-starting from vendor page</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>"- move 'upload' button to 'processed' page
@@ -219,13 +224,13 @@
 - on processing(downloading)  page of vendor, let's make two kinds of button. one is 'delevered', another is 'return/cancel'.
 - to do that, we add check box on each order item.  Default value is set as 'delivered'.
 - 'return/cancel' order is automatically return to the customer and relevant charges refund to his account.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">very important!!!!
 - this will change some relevant code of order and settlement from customer, vendor and admin. 
 </t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Check client &amp; server side validation in Profile page</t>
@@ -267,18 +272,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="나눔고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="나눔고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -301,6 +299,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="나눔고딕"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="나눔고딕"/>
     </font>
   </fonts>
@@ -326,24 +330,27 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -405,7 +412,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -437,9 +444,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -471,6 +479,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -646,11 +655,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -662,291 +671,297 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="59.25" customHeight="1">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="48.75" customHeight="1">
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="39.75" customHeight="1">
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="39.75" customHeight="1">
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="44.25" customHeight="1">
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="49.5" customHeight="1">
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="2:5" ht="44.25" customHeight="1">
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="66" customHeight="1">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="2:5" ht="59.25" customHeight="1">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="2:5" ht="42.75" customHeight="1">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="57" customHeight="1">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="45" customHeight="1">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="6" t="s">
         <v>24</v>
       </c>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="2:5" ht="45.75" customHeight="1">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="219.75" customHeight="1">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="25.5" customHeight="1">
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="72.75" customHeight="1">
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="28.5">
-      <c r="B19" s="1" t="s">
+    <row r="19" spans="2:5" ht="31.5">
+      <c r="B19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="4" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A1" s="5">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="15.75">
+      <c r="A1" s="3">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A2" s="5">
+    <row r="2" spans="1:10" s="3" customFormat="1" ht="15.75">
+      <c r="A2" s="3">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A3" s="5">
+    <row r="3" spans="1:10" s="3" customFormat="1" ht="15.75">
+      <c r="A3" s="3">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A4" s="5">
+    <row r="4" spans="1:10" s="3" customFormat="1" ht="15.75">
+      <c r="A4" s="3">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5">
+    <row r="5" spans="1:10" ht="15.75">
+      <c r="A5" s="3">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6">
+    <row r="6" spans="1:10" ht="15.75">
+      <c r="A6" s="3">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7">
+    <row r="7" spans="1:10" ht="15.75">
+      <c r="A7" s="3">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>54</v>
       </c>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
@@ -964,30 +979,30 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A10" s="5">
+    <row r="10" spans="1:10" s="3" customFormat="1" ht="15.75">
+      <c r="A10" s="3">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>